<commit_message>
Implement Markov-Approach for Intra-Day Storage
</commit_message>
<xml_diff>
--- a/data/NREL-118 7 clusters/Power_Parameters.xlsx
+++ b/data/NREL-118 7 clusters/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\NREL-118 7 clusters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723FA07E-1A32-4192-A315-A39C25F0709F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AF2168-74C4-4010-A3E1-BF3CE491E562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50190" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11790" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="93">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>bus001</t>
+  </si>
+  <si>
+    <t>Intra-Day Storage constraint type for edge timesteps</t>
+  </si>
+  <si>
+    <t>pReprPeriodEdgeHandlingIntraDayStorage</t>
   </si>
 </sst>
 </file>
@@ -554,7 +560,21 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1096,7 +1116,7 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H76"/>
+  <dimension ref="B1:H79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1687,16 +1707,46 @@
         <v>70</v>
       </c>
     </row>
+    <row r="78" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C6 C14:C28">
-    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
+    <cfRule type="cellIs" dxfId="31" priority="101" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="102" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:C12">
     <cfRule type="cellIs" dxfId="29" priority="99" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1704,23 +1754,23 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="27" priority="97" operator="equal">
+  <conditionalFormatting sqref="C31">
+    <cfRule type="cellIs" dxfId="27" priority="111" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="98" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="25" priority="109" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="112" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="25" priority="89" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="90" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37 C40">
     <cfRule type="cellIs" dxfId="23" priority="87" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1728,7 +1778,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37 C40">
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="21" priority="85" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1736,7 +1786,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
+  <conditionalFormatting sqref="C46">
     <cfRule type="cellIs" dxfId="19" priority="83" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1744,7 +1794,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
+  <conditionalFormatting sqref="C49">
     <cfRule type="cellIs" dxfId="17" priority="81" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1752,47 +1802,47 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="15" priority="79" operator="equal">
+  <conditionalFormatting sqref="C53 C56">
+    <cfRule type="cellIs" dxfId="15" priority="45" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="80" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53 C56">
-    <cfRule type="cellIs" dxfId="13" priority="43" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="46" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C61">
-    <cfRule type="cellIs" dxfId="11" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="95" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="96" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:C64">
-    <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="33" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="34" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C67">
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="29" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="30" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C70">
+    <cfRule type="cellIs" dxfId="7" priority="25" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C73">
     <cfRule type="cellIs" dxfId="5" priority="23" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1800,15 +1850,15 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
-    <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
+  <conditionalFormatting sqref="C76">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C79">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1821,7 +1871,7 @@
       <formula1>"No, Yes"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C61 C64 C67 C70 C15:C28" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
-    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C60 C46 C63 C66 C69 C73 C76" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C60 C46 C63 C66 C69 C73 C76 C79" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1829,12 +1879,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1984,15 +2031,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2016,17 +2074,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>